<commit_message>
actualizacion de ingreso emp mensajero
</commit_message>
<xml_diff>
--- a/Files/Reporte_Kardex_adm/1/Kardex_suc_1.xlsx
+++ b/Files/Reporte_Kardex_adm/1/Kardex_suc_1.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
   <si>
-    <t>Cargador Inalámbrico Ringke Carga Rápida 10W</t>
+    <t>Estuche Ringke Fusion X Apple Iphone 7/8 - Negro</t>
   </si>
   <si>
     <t>CODIGO</t>
@@ -26,13 +26,13 @@
     <t>UBICACIÓN</t>
   </si>
   <si>
-    <t>2B</t>
+    <t>7B</t>
   </si>
   <si>
     <t>SKU</t>
   </si>
   <si>
-    <t>ACWC0001</t>
+    <t>IGSG0011</t>
   </si>
   <si>
     <t>EXISTENCIA</t>
@@ -44,7 +44,7 @@
     <t>HORA</t>
   </si>
   <si>
-    <t>DESCRIPCIÓN</t>
+    <t>DETALLE/N° VENTA</t>
   </si>
   <si>
     <t>ENTRADAS</t>
@@ -144,11 +144,11 @@
     <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
+    <xf xfId="0" fontId="0" numFmtId="18" fillId="0" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="0" numFmtId="15" fillId="0" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="18" fillId="0" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -484,10 +484,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -510,7 +510,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4">
-        <v>8809550349483</v>
+        <v>8809628565333</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
@@ -532,7 +532,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="1">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:5" customHeight="1" ht="25">
@@ -553,17 +553,62 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="7">
-        <v>44150</v>
-      </c>
-      <c r="B5" s="8">
-        <v>0.077962962962963</v>
-      </c>
-      <c r="C5"/>
-      <c r="D5" s="5">
-        <v>10</v>
-      </c>
-      <c r="E5" s="6"/>
+      <c r="A5" s="8">
+        <v>44139</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0.82565972222222</v>
+      </c>
+      <c r="C5">
+        <v>300098762</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="8">
+        <v>44139</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0.77010416666667</v>
+      </c>
+      <c r="C6">
+        <v>302159019</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="8">
+        <v>44139</v>
+      </c>
+      <c r="B7" s="7">
+        <v>0.77008101851852</v>
+      </c>
+      <c r="C7">
+        <v>302158968</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="8">
+        <v>44139</v>
+      </c>
+      <c r="B8" s="7">
+        <v>0.60262731481481</v>
+      </c>
+      <c r="C8"/>
+      <c r="D8" s="5">
+        <v>40</v>
+      </c>
+      <c r="E8" s="6"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
actualizacion correcion de errores cambios visuales en formularios y entrada por login de mensajero
</commit_message>
<xml_diff>
--- a/Files/Reporte_Kardex_adm/1/Kardex_suc_1.xlsx
+++ b/Files/Reporte_Kardex_adm/1/Kardex_suc_1.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
   <si>
-    <t>Estuche Ringke Fusion X Apple Iphone 7/8 - Negro</t>
+    <t>Estuche Spigen Samsung Galaxy Note 8 - Negro</t>
   </si>
   <si>
     <t>CODIGO</t>
@@ -26,13 +26,13 @@
     <t>UBICACIÓN</t>
   </si>
   <si>
-    <t>7B</t>
+    <t>2C</t>
   </si>
   <si>
     <t>SKU</t>
   </si>
   <si>
-    <t>IGSG0011</t>
+    <t>587CS22051</t>
   </si>
   <si>
     <t>EXISTENCIA</t>
@@ -484,10 +484,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -510,7 +510,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4">
-        <v>8809628565333</v>
+        <v>8808522199474</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
@@ -532,7 +532,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="1">
-        <v>37</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" customHeight="1" ht="25">
@@ -554,13 +554,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="8">
-        <v>44139</v>
+        <v>44158</v>
       </c>
       <c r="B5" s="7">
-        <v>0.82565972222222</v>
+        <v>0.014375</v>
       </c>
       <c r="C5">
-        <v>300098762</v>
+        <v>4172472869</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="6">
@@ -569,46 +569,16 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="8">
-        <v>44139</v>
+        <v>44155</v>
       </c>
       <c r="B6" s="7">
-        <v>0.77010416666667</v>
-      </c>
-      <c r="C6">
-        <v>302159019</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="8">
-        <v>44139</v>
-      </c>
-      <c r="B7" s="7">
-        <v>0.77008101851852</v>
-      </c>
-      <c r="C7">
-        <v>302158968</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="8">
-        <v>44139</v>
-      </c>
-      <c r="B8" s="7">
-        <v>0.60262731481481</v>
-      </c>
-      <c r="C8"/>
-      <c r="D8" s="5">
-        <v>40</v>
-      </c>
-      <c r="E8" s="6"/>
+        <v>0.64954861111111</v>
+      </c>
+      <c r="C6"/>
+      <c r="D6" s="5">
+        <v>6</v>
+      </c>
+      <c r="E6" s="6"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>